<commit_message>
finished implementing first wave of tests with newly refactored object structure
</commit_message>
<xml_diff>
--- a/Tests/1/Test_MultiRun1.xlsx
+++ b/Tests/1/Test_MultiRun1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -722,7 +722,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
@@ -2281,8 +2281,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N353"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2847,41 +2847,40 @@
         <v>37</v>
       </c>
       <c r="C14" s="21">
-        <f>C196</f>
+        <v>11.5</v>
+      </c>
+      <c r="D14" s="45">
+        <v>11.5</v>
+      </c>
+      <c r="E14" s="45">
+        <v>11.5</v>
+      </c>
+      <c r="F14" s="45">
+        <v>11.5</v>
+      </c>
+      <c r="G14" s="20">
+        <v>7</v>
+      </c>
+      <c r="H14" s="20">
+        <v>11.5</v>
+      </c>
+      <c r="I14" s="20">
+        <v>7</v>
+      </c>
+      <c r="J14" s="20">
+        <v>5</v>
+      </c>
+      <c r="K14" s="20">
         <v>10</v>
       </c>
-      <c r="D14" s="45">
-        <v>10</v>
-      </c>
-      <c r="E14" s="47">
-        <v>10</v>
-      </c>
-      <c r="F14" s="20">
-        <v>10</v>
-      </c>
-      <c r="G14" s="20">
-        <v>6</v>
-      </c>
-      <c r="H14" s="20">
-        <v>10</v>
-      </c>
-      <c r="I14" s="20">
-        <v>6</v>
-      </c>
-      <c r="J14" s="20">
-        <v>4</v>
-      </c>
-      <c r="K14" s="20">
-        <v>9</v>
-      </c>
       <c r="L14" s="20">
-        <v>10</v>
+        <v>11.5</v>
       </c>
       <c r="M14" s="20">
-        <v>10</v>
+        <v>11.5</v>
       </c>
       <c r="N14" s="20">
-        <v>10</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2890,40 +2889,40 @@
         <v>38</v>
       </c>
       <c r="C15" s="21">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D15" s="45">
-        <v>30</v>
-      </c>
-      <c r="E15" s="47">
-        <v>30</v>
-      </c>
-      <c r="F15" s="20">
-        <v>30</v>
-      </c>
-      <c r="G15" s="20">
-        <v>30</v>
-      </c>
-      <c r="H15" s="20">
-        <v>29</v>
-      </c>
-      <c r="I15" s="20">
-        <v>30</v>
-      </c>
-      <c r="J15" s="20">
-        <v>30</v>
-      </c>
-      <c r="K15" s="20">
-        <v>30</v>
-      </c>
-      <c r="L15" s="20">
-        <v>29</v>
-      </c>
-      <c r="M15" s="20">
-        <v>30</v>
-      </c>
-      <c r="N15" s="20">
-        <v>30</v>
+        <v>45</v>
+      </c>
+      <c r="E15" s="45">
+        <v>45</v>
+      </c>
+      <c r="F15" s="45">
+        <v>45</v>
+      </c>
+      <c r="G15" s="45">
+        <v>45</v>
+      </c>
+      <c r="H15" s="45">
+        <v>45</v>
+      </c>
+      <c r="I15" s="45">
+        <v>45</v>
+      </c>
+      <c r="J15" s="45">
+        <v>45</v>
+      </c>
+      <c r="K15" s="45">
+        <v>45</v>
+      </c>
+      <c r="L15" s="45">
+        <v>45</v>
+      </c>
+      <c r="M15" s="45">
+        <v>45</v>
+      </c>
+      <c r="N15" s="45">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -3235,41 +3234,40 @@
         <v>37</v>
       </c>
       <c r="C23" s="21">
-        <f>C291</f>
+        <v>5</v>
+      </c>
+      <c r="D23" s="45">
         <v>4</v>
       </c>
-      <c r="D23" s="45">
+      <c r="E23" s="47">
+        <v>8</v>
+      </c>
+      <c r="F23" s="20">
+        <v>6</v>
+      </c>
+      <c r="G23" s="20">
         <v>3</v>
       </c>
-      <c r="E23" s="47">
-        <v>7</v>
-      </c>
-      <c r="F23" s="20">
-        <v>5</v>
-      </c>
-      <c r="G23" s="20">
-        <v>2</v>
-      </c>
       <c r="H23" s="20">
+        <v>4</v>
+      </c>
+      <c r="I23" s="20">
+        <v>4</v>
+      </c>
+      <c r="J23" s="20">
         <v>3</v>
       </c>
-      <c r="I23" s="20">
+      <c r="K23" s="20">
+        <v>4</v>
+      </c>
+      <c r="L23" s="20">
+        <v>6</v>
+      </c>
+      <c r="M23" s="20">
+        <v>4</v>
+      </c>
+      <c r="N23" s="20">
         <v>3</v>
-      </c>
-      <c r="J23" s="20">
-        <v>2</v>
-      </c>
-      <c r="K23" s="20">
-        <v>3</v>
-      </c>
-      <c r="L23" s="20">
-        <v>5</v>
-      </c>
-      <c r="M23" s="20">
-        <v>3</v>
-      </c>
-      <c r="N23" s="20">
-        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -3624,40 +3622,40 @@
         <v>37</v>
       </c>
       <c r="C32" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>